<commit_message>
Feat: get Payout list report
</commit_message>
<xml_diff>
--- a/assets/payout-list.xlsx
+++ b/assets/payout-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\AppData\Local\Temp\scp15806\usr\share\nginx\html\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/Project/lib/momo-salary/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84B4056-AAB2-4F77-9776-C0D9EDFB374B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF0D605-D72E-3741-AB12-4CD13EC7AE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21900" windowHeight="13176" xr2:uid="{3BE29609-0B2E-4DF8-9874-9D7B258F23DF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21900" windowHeight="13180" xr2:uid="{3BE29609-0B2E-4DF8-9874-9D7B258F23DF}"/>
   </bookViews>
   <sheets>
     <sheet name="FILE" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>0909010101</t>
-  </si>
-  <si>
     <t>SĐT
 (Bắt buộc)
 (Tối đa 10 số)</t>
@@ -61,10 +56,13 @@
 (Tối đa 50 triệu, với dịch vụ đặc biệt là 100 triệu)</t>
   </si>
   <si>
-    <t>Nguyễn Văn A</t>
-  </si>
-  <si>
     <t>Trưởng phòng</t>
+  </si>
+  <si>
+    <t>0916968263</t>
+  </si>
+  <si>
+    <t>Diệp Mỹ Dương</t>
   </si>
 </sst>
 </file>
@@ -447,43 +445,43 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3">
         <v>30000</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>